<commit_message>
screenshots and build plugins
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/EmployeeDetails.xlsx
+++ b/src/test/resources/testData/EmployeeDetails.xlsx
@@ -42,40 +42,40 @@
     <t>confirmPassword</t>
   </si>
   <si>
-    <t>Poolik</t>
-  </si>
-  <si>
-    <t>Validoon</t>
-  </si>
-  <si>
-    <t>Feerasol</t>
-  </si>
-  <si>
     <t>MS</t>
   </si>
   <si>
-    <t>Deerakol</t>
-  </si>
-  <si>
-    <t>Rawiol</t>
-  </si>
-  <si>
-    <t>Pomeedor</t>
-  </si>
-  <si>
     <t>Syntax123!</t>
   </si>
   <si>
-    <t>Poolik123</t>
-  </si>
-  <si>
-    <t>Feerasol123</t>
-  </si>
-  <si>
-    <t>Rawiol123</t>
-  </si>
-  <si>
     <t>D:\employee_photo\my_photo.jpg</t>
+  </si>
+  <si>
+    <t>Derakoll</t>
+  </si>
+  <si>
+    <t>Pomedorr</t>
+  </si>
+  <si>
+    <t>Sapirtom</t>
+  </si>
+  <si>
+    <t>Bertokr</t>
+  </si>
+  <si>
+    <t>Weportt</t>
+  </si>
+  <si>
+    <t>Xeelopp</t>
+  </si>
+  <si>
+    <t>Xeelopp325</t>
+  </si>
+  <si>
+    <t>Weportt325</t>
+  </si>
+  <si>
+    <t>Bertokk325</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,71 +445,71 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>